<commit_message>
Minor updates to ParticipantsAndTasks.xlsx
</commit_message>
<xml_diff>
--- a/docs/ParticipantsAndTasks.xlsx
+++ b/docs/ParticipantsAndTasks.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="51">
   <si>
     <t>№ п/п</t>
   </si>
@@ -788,7 +788,7 @@
   <dimension ref="A2:F27"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -865,9 +865,15 @@
       <c r="A5" s="9">
         <v>3</v>
       </c>
-      <c r="B5" s="10"/>
-      <c r="C5" s="10"/>
-      <c r="D5" s="10"/>
+      <c r="B5" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5" s="10" t="s">
+        <v>8</v>
+      </c>
       <c r="E5" s="10" t="s">
         <v>9</v>
       </c>
@@ -879,9 +885,15 @@
       <c r="A6" s="9">
         <v>4</v>
       </c>
-      <c r="B6" s="10"/>
-      <c r="C6" s="10"/>
-      <c r="D6" s="10"/>
+      <c r="B6" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="D6" s="10" t="s">
+        <v>8</v>
+      </c>
       <c r="E6" s="10" t="s">
         <v>9</v>
       </c>
@@ -1190,6 +1202,7 @@
   <hyperlinks>
     <hyperlink ref="C3" r:id="rId1"/>
     <hyperlink ref="C4" r:id="rId2"/>
+    <hyperlink ref="C5:C6" r:id="rId3" display="chebotaryovnik@gmail.com"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>

</xml_diff>